<commit_message>
keynote speaker info added
</commit_message>
<xml_diff>
--- a/data/DHS2025_Agenda.xlsx
+++ b/data/DHS2025_Agenda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.novartis.net/personal/asokaar1_novartis_net/Documents/Personal/Work Personal/Conference/AV 2025/Agentic KAG/codes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{66C783D6-079A-42F9-A263-D437FB637739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F46D19B9-7887-46A8-9A61-924FD8A7E3CA}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{66C783D6-079A-42F9-A263-D437FB637739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EFF6A24-9315-44DA-B29D-F6467F0EDC18}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Agenda!$A$1:$H$95</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="215">
   <si>
     <t>Day</t>
   </si>
@@ -659,6 +672,15 @@
   </si>
   <si>
     <t>Architecting AI: Practical Patterns for Multi-Agentic Workflows</t>
+  </si>
+  <si>
+    <t>Evolution of Intelligence &amp; You</t>
+  </si>
+  <si>
+    <t>Agentic AI for Business Users: Building without Code in Cogentiq</t>
+  </si>
+  <si>
+    <t>Ganesh Subramanian</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,7 +1311,7 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>212</v>
       </c>
       <c r="H10" t="s">
         <v>151</v>
@@ -3095,10 +3117,10 @@
         <v>27</v>
       </c>
       <c r="G82" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="H82" t="s">
-        <v>90</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>